<commit_message>
Use nanotime instead of milliseconds
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -78,10 +78,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,13 +120,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,11 +472,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="1849689376"/>
-        <c:axId val="1850466320"/>
+        <c:axId val="-1678327024"/>
+        <c:axId val="-1678323664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1849689376"/>
+        <c:axId val="-1678327024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -571,7 +591,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1850466320"/>
+        <c:crossAx val="-1678323664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -579,7 +599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1850466320"/>
+        <c:axId val="-1678323664"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -695,7 +715,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1849689376"/>
+        <c:crossAx val="-1678327024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1101,11 +1121,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="1848378736"/>
-        <c:axId val="1828169920"/>
+        <c:axId val="-1678297632"/>
+        <c:axId val="-1678293600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1848378736"/>
+        <c:axId val="-1678297632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1220,7 +1240,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1828169920"/>
+        <c:crossAx val="-1678293600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1228,7 +1248,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1828169920"/>
+        <c:axId val="-1678293600"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1343,7 +1363,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1848378736"/>
+        <c:crossAx val="-1678297632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1469,7 +1489,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Client.sleep: 10ms, Server.sleep: 250ms</a:t>
+              <a:t>Client.sleep: 25ms, Server.sleep: 250ms</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1749,11 +1769,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="1827630576"/>
-        <c:axId val="1849261808"/>
+        <c:axId val="-1678264480"/>
+        <c:axId val="-1678260448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1827630576"/>
+        <c:axId val="-1678264480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1868,7 +1888,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1849261808"/>
+        <c:crossAx val="-1678260448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1876,7 +1896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1849261808"/>
+        <c:axId val="-1678260448"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1991,7 +2011,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1827630576"/>
+        <c:crossAx val="-1678264480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2124,7 +2144,7 @@
               <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Client.sleep: 10ms, Server.sleep: 250ms</a:t>
+              <a:t>Client.sleep: 25ms, Server.sleep: 250ms</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100">
               <a:effectLst/>
@@ -2413,11 +2433,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="1888898160"/>
-        <c:axId val="1888899520"/>
+        <c:axId val="-1678233200"/>
+        <c:axId val="-1678229168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1888898160"/>
+        <c:axId val="-1678233200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2532,7 +2552,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888899520"/>
+        <c:crossAx val="-1678229168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2540,7 +2560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1888899520"/>
+        <c:axId val="-1678229168"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2660,7 +2680,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888898160"/>
+        <c:crossAx val="-1678233200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3048,11 +3068,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="1853517280"/>
-        <c:axId val="1890177264"/>
+        <c:axId val="-1678199344"/>
+        <c:axId val="-1678195312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1853517280"/>
+        <c:axId val="-1678199344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3167,7 +3187,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1890177264"/>
+        <c:crossAx val="-1678195312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3175,7 +3195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1890177264"/>
+        <c:axId val="-1678195312"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3290,7 +3310,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1853517280"/>
+        <c:crossAx val="-1678199344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3409,7 +3429,7 @@
               <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Single-Threaded Server</a:t>
+              <a:t>Multi-Threaded Server</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100">
               <a:effectLst/>
@@ -3688,11 +3708,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="1889450832"/>
-        <c:axId val="1889442160"/>
+        <c:axId val="-1720300736"/>
+        <c:axId val="-1678163232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1889450832"/>
+        <c:axId val="-1720300736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3807,7 +3827,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1889442160"/>
+        <c:crossAx val="-1678163232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3815,7 +3835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1889442160"/>
+        <c:axId val="-1678163232"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3931,7 +3951,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1889450832"/>
+        <c:crossAx val="-1720300736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7998,8 +8018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>